<commit_message>
add requirements.txt + ascii filenames for theses
</commit_message>
<xml_diff>
--- a/static/data/theses_inventory.xlsx
+++ b/static/data/theses_inventory.xlsx
@@ -95,7 +95,7 @@
     <t>Lost in Translation: Analyzing Machine Translation Quality Estimation with Synthetic Challenges</t>
   </si>
   <si>
-    <t>thesis_Selin_Açikel_2024.pdf</t>
+    <t>thesis_Selin_Acikel_2024.pdf</t>
   </si>
   <si>
     <t>no</t>
@@ -116,7 +116,7 @@
     <t>Multi-Label Topic Classification of Client Feedback in the Governance Domain</t>
   </si>
   <si>
-    <t>thesis_Csenge_Szabó_2024.pdf</t>
+    <t>thesis_Csenge_Szabo_2024.pdf</t>
   </si>
   <si>
     <t>Payam Fakhraei</t>
@@ -563,7 +563,7 @@
     <t>Automatic Generation of Personalized Counter Narratives Based on User Profile</t>
   </si>
   <si>
-    <t>thesis_Mekselina_Doğanç_2023.pdf</t>
+    <t>thesis_Mekselina_Doganc_2023.pdf</t>
   </si>
   <si>
     <t>Mojca Kloos</t>
@@ -1165,7 +1165,7 @@
       <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -3171,7 +3171,7 @@
       <c r="C8" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>181</v>
       </c>
       <c r="E8" s="2" t="s">

</xml_diff>